<commit_message>
Iteration 5 Closeout Files
</commit_message>
<xml_diff>
--- a/Group 11 Estimation.xlsx
+++ b/Group 11 Estimation.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="96">
   <si>
     <t>Task Name: (Dependencies top to bottom)</t>
   </si>
@@ -307,7 +307,10 @@
     <t>Iteration 5</t>
   </si>
   <si>
-    <t>Build Scheduler, and course adding</t>
+    <t>Build Scheduler, and professors adding</t>
+  </si>
+  <si>
+    <t>Blake, Ray</t>
   </si>
   <si>
     <t>Complete SQLite Database</t>
@@ -323,7 +326,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="15">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -385,6 +388,7 @@
       <name val="Arial"/>
     </font>
     <font>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -392,28 +396,13 @@
       <name val="Arial"/>
     </font>
     <font>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b/>
       <sz val="10.0"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10.0"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10.0"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12.0"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="7">
@@ -722,7 +711,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="244">
+  <cellXfs count="243">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1317,11 +1306,14 @@
     <xf borderId="22" fillId="3" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="25" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="22" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="20" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="25" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="26" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -1332,6 +1324,9 @@
     <xf borderId="21" fillId="4" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="21" fillId="4" fontId="11" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="27" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="27" fillId="4" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyFont="1"/>
@@ -1348,8 +1343,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="11" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="5" fontId="13" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="22" fillId="5" fontId="9" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="22" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -1362,68 +1363,53 @@
     <xf borderId="22" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="22" fillId="4" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf borderId="0" fillId="4" fontId="11" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="22" fillId="4" fontId="11" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="5" fontId="12" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="22" fillId="5" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="22" fillId="5" fontId="12" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="26" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="26" fillId="5" fontId="11" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="29" fillId="6" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="29" fillId="6" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="30" fillId="6" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="30" fillId="6" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="31" fillId="6" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="31" fillId="6" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="29" fillId="6" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="29" fillId="6" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="10" fillId="6" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="6" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="29" fillId="6" fontId="13" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="29" fillId="6" fontId="14" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4850,7 +4836,7 @@
       <c r="H66" s="193"/>
       <c r="I66" s="176">
         <f>SUM(H67:H70)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J66" s="177"/>
       <c r="K66" s="177"/>
@@ -5042,7 +5028,7 @@
       <c r="G70" s="185"/>
       <c r="H70" s="186">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I70" s="187"/>
       <c r="J70" s="177"/>
@@ -5055,10 +5041,12 @@
       </c>
       <c r="N70" s="189"/>
       <c r="O70" s="189"/>
-      <c r="P70" s="189"/>
+      <c r="P70" s="190">
+        <v>1.0</v>
+      </c>
       <c r="Q70" s="197">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R70" s="177"/>
       <c r="S70" s="177"/>
@@ -5090,9 +5078,9 @@
         <v>4</v>
       </c>
       <c r="H71" s="193"/>
-      <c r="I71" s="176">
+      <c r="I71" s="198">
         <f>SUM(H72:H73)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J71" s="177"/>
       <c r="K71" s="177"/>
@@ -5134,9 +5122,8 @@
         <v>2.0</v>
       </c>
       <c r="G72" s="185"/>
-      <c r="H72" s="186">
-        <f>Q72</f>
-        <v>0</v>
+      <c r="H72" s="199">
+        <v>2.0</v>
       </c>
       <c r="I72" s="187"/>
       <c r="J72" s="177"/>
@@ -5145,7 +5132,9 @@
       <c r="M72" s="189"/>
       <c r="N72" s="189"/>
       <c r="O72" s="189"/>
-      <c r="P72" s="189"/>
+      <c r="P72" s="190">
+        <v>1.0</v>
+      </c>
       <c r="Q72" s="197">
         <f t="shared" ref="Q72:Q73" si="15">SUM(L71:P71)</f>
         <v>0</v>
@@ -5181,21 +5170,23 @@
       <c r="F73" s="183">
         <v>2.0</v>
       </c>
-      <c r="G73" s="198"/>
+      <c r="G73" s="200"/>
       <c r="H73" s="199">
-        <v>1.0</v>
-      </c>
-      <c r="I73" s="200"/>
+        <v>2.0</v>
+      </c>
+      <c r="I73" s="201"/>
       <c r="J73" s="177"/>
       <c r="K73" s="177"/>
       <c r="L73" s="188"/>
       <c r="M73" s="189"/>
       <c r="N73" s="189"/>
       <c r="O73" s="189"/>
-      <c r="P73" s="189"/>
+      <c r="P73" s="190">
+        <v>1.0</v>
+      </c>
       <c r="Q73" s="197">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R73" s="177"/>
       <c r="S73" s="177"/>
@@ -5214,33 +5205,33 @@
       <c r="AF73" s="177"/>
     </row>
     <row r="74" ht="12.75" customHeight="1">
-      <c r="A74" s="201" t="s">
+      <c r="A74" s="202" t="s">
         <v>91</v>
       </c>
-      <c r="B74" s="202" t="s">
+      <c r="B74" s="203" t="s">
         <v>61</v>
       </c>
-      <c r="C74" s="203"/>
-      <c r="D74" s="203"/>
-      <c r="E74" s="203"/>
-      <c r="F74" s="203"/>
-      <c r="G74" s="204">
+      <c r="C74" s="204"/>
+      <c r="D74" s="204"/>
+      <c r="E74" s="204"/>
+      <c r="F74" s="204"/>
+      <c r="G74" s="205">
         <f>SUM(F75:F77)</f>
-        <v>5</v>
-      </c>
-      <c r="H74" s="203"/>
-      <c r="I74" s="204">
+        <v>4</v>
+      </c>
+      <c r="H74" s="204"/>
+      <c r="I74" s="206">
         <f>SUM(H75:H77)</f>
-        <v>0</v>
-      </c>
-      <c r="J74" s="205"/>
-      <c r="K74" s="206"/>
-      <c r="L74" s="207"/>
-      <c r="M74" s="207"/>
-      <c r="N74" s="207"/>
-      <c r="O74" s="207"/>
-      <c r="P74" s="207"/>
-      <c r="Q74" s="208"/>
+        <v>4</v>
+      </c>
+      <c r="J74" s="207"/>
+      <c r="K74" s="208"/>
+      <c r="L74" s="209"/>
+      <c r="M74" s="209"/>
+      <c r="N74" s="209"/>
+      <c r="O74" s="209"/>
+      <c r="P74" s="209"/>
+      <c r="Q74" s="210"/>
       <c r="R74" s="177"/>
       <c r="S74" s="177"/>
       <c r="T74" s="177"/>
@@ -5258,33 +5249,38 @@
       <c r="AF74" s="177"/>
     </row>
     <row r="75" ht="12.75" customHeight="1">
-      <c r="A75" s="209"/>
-      <c r="B75" s="210"/>
-      <c r="C75" s="211" t="s">
+      <c r="A75" s="211"/>
+      <c r="B75" s="212"/>
+      <c r="C75" s="213" t="s">
         <v>62</v>
       </c>
-      <c r="D75" s="212" t="s">
+      <c r="D75" s="214" t="s">
         <v>19</v>
       </c>
-      <c r="E75" s="213" t="s">
+      <c r="E75" s="215" t="s">
         <v>3</v>
       </c>
-      <c r="F75" s="212">
+      <c r="F75" s="214">
         <v>1.0</v>
       </c>
-      <c r="G75" s="209"/>
-      <c r="H75" s="210"/>
-      <c r="I75" s="209"/>
-      <c r="J75" s="205"/>
-      <c r="K75" s="206"/>
-      <c r="L75" s="214"/>
-      <c r="M75" s="214"/>
-      <c r="N75" s="214"/>
-      <c r="O75" s="214"/>
-      <c r="P75" s="214"/>
-      <c r="Q75" s="215">
-        <f t="shared" ref="Q75:Q77" si="16">SUM(L75:P75)</f>
-        <v>0</v>
+      <c r="G75" s="211"/>
+      <c r="H75" s="216">
+        <f t="shared" ref="H75:H77" si="16">Q75</f>
+        <v>2</v>
+      </c>
+      <c r="I75" s="211"/>
+      <c r="J75" s="207"/>
+      <c r="K75" s="208"/>
+      <c r="L75" s="216"/>
+      <c r="M75" s="216"/>
+      <c r="N75" s="217">
+        <v>2.0</v>
+      </c>
+      <c r="O75" s="216"/>
+      <c r="P75" s="216"/>
+      <c r="Q75" s="218">
+        <f t="shared" ref="Q75:Q77" si="17">SUM(L75:P75)</f>
+        <v>2</v>
       </c>
       <c r="R75" s="177"/>
       <c r="S75" s="177"/>
@@ -5303,33 +5299,38 @@
       <c r="AF75" s="177"/>
     </row>
     <row r="76" ht="12.75" customHeight="1">
-      <c r="A76" s="209"/>
-      <c r="B76" s="210"/>
-      <c r="C76" s="211" t="s">
+      <c r="A76" s="211"/>
+      <c r="B76" s="212"/>
+      <c r="C76" s="213" t="s">
         <v>63</v>
       </c>
-      <c r="D76" s="212" t="s">
+      <c r="D76" s="214" t="s">
         <v>19</v>
       </c>
-      <c r="E76" s="213" t="s">
+      <c r="E76" s="215" t="s">
         <v>3</v>
       </c>
-      <c r="F76" s="212">
+      <c r="F76" s="214">
         <v>2.0</v>
       </c>
-      <c r="G76" s="209"/>
-      <c r="H76" s="210"/>
-      <c r="I76" s="209"/>
-      <c r="J76" s="205"/>
-      <c r="K76" s="206"/>
-      <c r="L76" s="214"/>
-      <c r="M76" s="214"/>
-      <c r="N76" s="214"/>
-      <c r="O76" s="214"/>
-      <c r="P76" s="214"/>
-      <c r="Q76" s="215">
+      <c r="G76" s="211"/>
+      <c r="H76" s="216">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="I76" s="211"/>
+      <c r="J76" s="207"/>
+      <c r="K76" s="208"/>
+      <c r="L76" s="216"/>
+      <c r="M76" s="216"/>
+      <c r="N76" s="217">
+        <v>2.0</v>
+      </c>
+      <c r="O76" s="216"/>
+      <c r="P76" s="216"/>
+      <c r="Q76" s="218">
+        <f t="shared" si="17"/>
+        <v>2</v>
       </c>
       <c r="R76" s="177"/>
       <c r="S76" s="177"/>
@@ -5348,37 +5349,36 @@
       <c r="AF76" s="177"/>
     </row>
     <row r="77" ht="12.75" customHeight="1">
-      <c r="A77" s="209"/>
-      <c r="B77" s="210"/>
-      <c r="C77" s="211" t="s">
+      <c r="A77" s="211"/>
+      <c r="B77" s="212"/>
+      <c r="C77" s="213" t="s">
         <v>76</v>
       </c>
-      <c r="D77" s="212" t="s">
+      <c r="D77" s="214" t="s">
         <v>42</v>
       </c>
-      <c r="E77" s="213" t="s">
+      <c r="E77" s="215" t="s">
         <v>1</v>
       </c>
-      <c r="F77" s="212">
-        <v>2.0</v>
-      </c>
-      <c r="G77" s="216">
+      <c r="F77" s="219">
         <v>1.0</v>
       </c>
-      <c r="H77" s="210"/>
-      <c r="I77" s="209"/>
-      <c r="J77" s="205"/>
-      <c r="K77" s="206"/>
-      <c r="L77" s="217">
-        <v>1.0</v>
-      </c>
-      <c r="M77" s="214"/>
-      <c r="N77" s="214"/>
-      <c r="O77" s="214"/>
-      <c r="P77" s="214"/>
-      <c r="Q77" s="215">
+      <c r="G77" s="220"/>
+      <c r="H77" s="216">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I77" s="211"/>
+      <c r="J77" s="207"/>
+      <c r="K77" s="208"/>
+      <c r="L77" s="221"/>
+      <c r="M77" s="216"/>
+      <c r="N77" s="216"/>
+      <c r="O77" s="216"/>
+      <c r="P77" s="216"/>
+      <c r="Q77" s="218">
+        <f t="shared" si="17"/>
+        <v>0</v>
       </c>
       <c r="R77" s="177"/>
       <c r="S77" s="177"/>
@@ -5397,31 +5397,31 @@
       <c r="AF77" s="177"/>
     </row>
     <row r="78" ht="12.75" customHeight="1">
-      <c r="A78" s="209"/>
-      <c r="B78" s="218" t="s">
+      <c r="A78" s="211"/>
+      <c r="B78" s="222" t="s">
         <v>40</v>
       </c>
-      <c r="C78" s="219"/>
-      <c r="D78" s="219"/>
-      <c r="E78" s="219"/>
-      <c r="F78" s="219"/>
-      <c r="G78" s="220">
+      <c r="C78" s="223"/>
+      <c r="D78" s="223"/>
+      <c r="E78" s="223"/>
+      <c r="F78" s="223"/>
+      <c r="G78" s="224">
         <f>SUM(F79:F82)</f>
-        <v>22</v>
-      </c>
-      <c r="H78" s="219"/>
-      <c r="I78" s="220">
+        <v>21</v>
+      </c>
+      <c r="H78" s="223"/>
+      <c r="I78" s="225">
         <f>SUM(H79:H82)</f>
-        <v>0</v>
-      </c>
-      <c r="J78" s="205"/>
-      <c r="K78" s="206"/>
-      <c r="L78" s="221"/>
-      <c r="M78" s="221"/>
-      <c r="N78" s="221"/>
-      <c r="O78" s="221"/>
-      <c r="P78" s="221"/>
-      <c r="Q78" s="222"/>
+        <v>18</v>
+      </c>
+      <c r="J78" s="207"/>
+      <c r="K78" s="208"/>
+      <c r="L78" s="226"/>
+      <c r="M78" s="226"/>
+      <c r="N78" s="226"/>
+      <c r="O78" s="226"/>
+      <c r="P78" s="226"/>
+      <c r="Q78" s="227"/>
       <c r="R78" s="177"/>
       <c r="S78" s="177"/>
       <c r="T78" s="177"/>
@@ -5439,37 +5439,38 @@
       <c r="AF78" s="177"/>
     </row>
     <row r="79" ht="12.75" customHeight="1">
-      <c r="A79" s="209"/>
-      <c r="B79" s="210"/>
-      <c r="C79" s="211" t="s">
+      <c r="A79" s="211"/>
+      <c r="B79" s="212"/>
+      <c r="C79" s="213" t="s">
         <v>85</v>
       </c>
-      <c r="D79" s="212" t="s">
+      <c r="D79" s="214" t="s">
         <v>42</v>
       </c>
-      <c r="E79" s="213" t="s">
+      <c r="E79" s="215" t="s">
         <v>1</v>
       </c>
-      <c r="F79" s="212">
-        <v>4.0</v>
-      </c>
-      <c r="G79" s="216">
+      <c r="F79" s="219">
         <v>3.0</v>
       </c>
-      <c r="H79" s="210"/>
-      <c r="I79" s="209"/>
-      <c r="J79" s="205"/>
-      <c r="K79" s="206"/>
-      <c r="L79" s="217">
-        <v>6.0</v>
-      </c>
-      <c r="M79" s="214"/>
-      <c r="N79" s="214"/>
-      <c r="O79" s="214"/>
-      <c r="P79" s="214"/>
-      <c r="Q79" s="215">
-        <f t="shared" ref="Q79:Q82" si="17">SUM(L79:P79)</f>
-        <v>6</v>
+      <c r="G79" s="220"/>
+      <c r="H79" s="216">
+        <f t="shared" ref="H79:H81" si="18">Q79</f>
+        <v>2</v>
+      </c>
+      <c r="I79" s="211"/>
+      <c r="J79" s="207"/>
+      <c r="K79" s="208"/>
+      <c r="L79" s="228">
+        <v>2.0</v>
+      </c>
+      <c r="M79" s="216"/>
+      <c r="N79" s="216"/>
+      <c r="O79" s="216"/>
+      <c r="P79" s="216"/>
+      <c r="Q79" s="218">
+        <f t="shared" ref="Q79:Q82" si="19">SUM(L79:P79)</f>
+        <v>2</v>
       </c>
       <c r="R79" s="177"/>
       <c r="S79" s="177"/>
@@ -5488,33 +5489,40 @@
       <c r="AF79" s="177"/>
     </row>
     <row r="80" ht="12.75" customHeight="1">
-      <c r="A80" s="209"/>
-      <c r="B80" s="210"/>
-      <c r="C80" s="223" t="s">
+      <c r="A80" s="211"/>
+      <c r="B80" s="212"/>
+      <c r="C80" s="229" t="s">
         <v>92</v>
       </c>
-      <c r="D80" s="212" t="s">
+      <c r="D80" s="214" t="s">
         <v>42</v>
       </c>
-      <c r="E80" s="213" t="s">
-        <v>2</v>
-      </c>
-      <c r="F80" s="224">
-        <v>10.0</v>
-      </c>
-      <c r="G80" s="209"/>
-      <c r="H80" s="210"/>
-      <c r="I80" s="209"/>
-      <c r="J80" s="205"/>
-      <c r="K80" s="206"/>
-      <c r="L80" s="214"/>
-      <c r="M80" s="214"/>
-      <c r="N80" s="214"/>
-      <c r="O80" s="214"/>
-      <c r="P80" s="214"/>
-      <c r="Q80" s="215">
-        <f t="shared" si="17"/>
-        <v>0</v>
+      <c r="E80" s="230" t="s">
+        <v>93</v>
+      </c>
+      <c r="F80" s="219">
+        <v>12.0</v>
+      </c>
+      <c r="G80" s="231"/>
+      <c r="H80" s="216">
+        <f t="shared" si="18"/>
+        <v>12</v>
+      </c>
+      <c r="I80" s="211"/>
+      <c r="J80" s="207"/>
+      <c r="K80" s="208"/>
+      <c r="L80" s="216"/>
+      <c r="M80" s="217">
+        <v>8.0</v>
+      </c>
+      <c r="N80" s="216"/>
+      <c r="O80" s="216"/>
+      <c r="P80" s="217">
+        <v>4.0</v>
+      </c>
+      <c r="Q80" s="218">
+        <f t="shared" si="19"/>
+        <v>12</v>
       </c>
       <c r="R80" s="177"/>
       <c r="S80" s="177"/>
@@ -5533,33 +5541,38 @@
       <c r="AF80" s="177"/>
     </row>
     <row r="81" ht="12.75" customHeight="1">
-      <c r="A81" s="209"/>
-      <c r="B81" s="210"/>
-      <c r="C81" s="223" t="s">
-        <v>93</v>
-      </c>
-      <c r="D81" s="212" t="s">
+      <c r="A81" s="211"/>
+      <c r="B81" s="212"/>
+      <c r="C81" s="229" t="s">
+        <v>94</v>
+      </c>
+      <c r="D81" s="214" t="s">
         <v>42</v>
       </c>
-      <c r="E81" s="225" t="s">
-        <v>94</v>
-      </c>
-      <c r="F81" s="212">
+      <c r="E81" s="230" t="s">
+        <v>95</v>
+      </c>
+      <c r="F81" s="214">
         <v>4.0</v>
       </c>
-      <c r="G81" s="209"/>
-      <c r="H81" s="210"/>
-      <c r="I81" s="209"/>
-      <c r="J81" s="205"/>
-      <c r="K81" s="206"/>
-      <c r="L81" s="214"/>
-      <c r="M81" s="214"/>
-      <c r="N81" s="214"/>
-      <c r="O81" s="214"/>
-      <c r="P81" s="214"/>
-      <c r="Q81" s="226">
-        <f t="shared" si="17"/>
-        <v>0</v>
+      <c r="G81" s="231"/>
+      <c r="H81" s="216">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="I81" s="211"/>
+      <c r="J81" s="207"/>
+      <c r="K81" s="208"/>
+      <c r="L81" s="216"/>
+      <c r="M81" s="217">
+        <v>1.0</v>
+      </c>
+      <c r="N81" s="216"/>
+      <c r="O81" s="216"/>
+      <c r="P81" s="216"/>
+      <c r="Q81" s="232">
+        <f t="shared" si="19"/>
+        <v>1</v>
       </c>
       <c r="R81" s="177"/>
       <c r="S81" s="177"/>
@@ -5578,37 +5591,39 @@
       <c r="AF81" s="177"/>
     </row>
     <row r="82" ht="12.75" customHeight="1">
-      <c r="A82" s="209"/>
-      <c r="B82" s="210"/>
-      <c r="C82" s="211" t="s">
+      <c r="A82" s="211"/>
+      <c r="B82" s="212"/>
+      <c r="C82" s="213" t="s">
         <v>87</v>
       </c>
-      <c r="D82" s="212" t="s">
+      <c r="D82" s="214" t="s">
         <v>42</v>
       </c>
-      <c r="E82" s="213" t="s">
+      <c r="E82" s="215" t="s">
         <v>88</v>
       </c>
-      <c r="F82" s="212">
-        <v>4.0</v>
-      </c>
-      <c r="G82" s="216">
+      <c r="F82" s="219">
         <v>2.0</v>
       </c>
-      <c r="H82" s="210"/>
-      <c r="I82" s="209"/>
-      <c r="J82" s="205"/>
-      <c r="K82" s="206"/>
-      <c r="L82" s="217">
+      <c r="G82" s="231"/>
+      <c r="H82" s="233">
+        <v>3.0</v>
+      </c>
+      <c r="I82" s="211"/>
+      <c r="J82" s="207"/>
+      <c r="K82" s="208"/>
+      <c r="L82" s="221"/>
+      <c r="M82" s="217">
+        <v>2.0</v>
+      </c>
+      <c r="N82" s="216"/>
+      <c r="O82" s="216"/>
+      <c r="P82" s="217">
         <v>1.0</v>
       </c>
-      <c r="M82" s="214"/>
-      <c r="N82" s="214"/>
-      <c r="O82" s="214"/>
-      <c r="P82" s="214"/>
-      <c r="Q82" s="226">
-        <f t="shared" si="17"/>
-        <v>1</v>
+      <c r="Q82" s="232">
+        <f t="shared" si="19"/>
+        <v>3</v>
       </c>
       <c r="R82" s="177"/>
       <c r="S82" s="177"/>
@@ -5627,31 +5642,31 @@
       <c r="AF82" s="177"/>
     </row>
     <row r="83" ht="12.75" customHeight="1">
-      <c r="A83" s="209"/>
-      <c r="B83" s="218" t="s">
+      <c r="A83" s="211"/>
+      <c r="B83" s="222" t="s">
         <v>55</v>
       </c>
-      <c r="C83" s="219"/>
-      <c r="D83" s="219"/>
-      <c r="E83" s="219"/>
-      <c r="F83" s="219"/>
-      <c r="G83" s="220">
+      <c r="C83" s="223"/>
+      <c r="D83" s="223"/>
+      <c r="E83" s="223"/>
+      <c r="F83" s="223"/>
+      <c r="G83" s="224">
         <f>SUM(F84:F85)</f>
         <v>4</v>
       </c>
-      <c r="H83" s="219"/>
-      <c r="I83" s="220">
+      <c r="H83" s="223"/>
+      <c r="I83" s="224">
         <f>SUM(H84:H85)</f>
-        <v>0</v>
-      </c>
-      <c r="J83" s="205"/>
-      <c r="K83" s="206"/>
-      <c r="L83" s="221"/>
-      <c r="M83" s="221"/>
-      <c r="N83" s="221"/>
-      <c r="O83" s="221"/>
-      <c r="P83" s="221"/>
-      <c r="Q83" s="222"/>
+        <v>4</v>
+      </c>
+      <c r="J83" s="207"/>
+      <c r="K83" s="208"/>
+      <c r="L83" s="226"/>
+      <c r="M83" s="226"/>
+      <c r="N83" s="226"/>
+      <c r="O83" s="226"/>
+      <c r="P83" s="226"/>
+      <c r="Q83" s="227"/>
       <c r="R83" s="177"/>
       <c r="S83" s="177"/>
       <c r="T83" s="177"/>
@@ -5669,32 +5684,36 @@
       <c r="AF83" s="177"/>
     </row>
     <row r="84" ht="12.75" customHeight="1">
-      <c r="A84" s="209"/>
-      <c r="B84" s="210"/>
-      <c r="C84" s="211" t="s">
+      <c r="A84" s="211"/>
+      <c r="B84" s="212"/>
+      <c r="C84" s="213" t="s">
         <v>82</v>
       </c>
-      <c r="D84" s="212" t="s">
+      <c r="D84" s="214" t="s">
         <v>83</v>
       </c>
-      <c r="E84" s="213" t="s">
+      <c r="E84" s="215" t="s">
         <v>89</v>
       </c>
-      <c r="F84" s="212">
+      <c r="F84" s="214">
         <v>2.0</v>
       </c>
-      <c r="G84" s="209"/>
-      <c r="H84" s="210"/>
-      <c r="I84" s="209"/>
-      <c r="J84" s="205"/>
-      <c r="K84" s="206"/>
-      <c r="L84" s="214"/>
-      <c r="M84" s="214"/>
-      <c r="N84" s="214"/>
-      <c r="O84" s="214"/>
-      <c r="P84" s="214"/>
-      <c r="Q84" s="226">
-        <f t="shared" ref="Q84:Q85" si="18">SUM(L83:P83)</f>
+      <c r="G84" s="211"/>
+      <c r="H84" s="233">
+        <v>2.0</v>
+      </c>
+      <c r="I84" s="211"/>
+      <c r="J84" s="207"/>
+      <c r="K84" s="208"/>
+      <c r="L84" s="216"/>
+      <c r="M84" s="216"/>
+      <c r="N84" s="216"/>
+      <c r="O84" s="216"/>
+      <c r="P84" s="217">
+        <v>1.0</v>
+      </c>
+      <c r="Q84" s="232">
+        <f t="shared" ref="Q84:Q85" si="20">SUM(L83:P83)</f>
         <v>0</v>
       </c>
       <c r="R84" s="177"/>
@@ -5714,35 +5733,39 @@
       <c r="AF84" s="177"/>
     </row>
     <row r="85" ht="12.75" customHeight="1">
-      <c r="A85" s="209"/>
-      <c r="B85" s="210"/>
-      <c r="C85" s="211" t="s">
+      <c r="A85" s="211"/>
+      <c r="B85" s="212"/>
+      <c r="C85" s="213" t="s">
         <v>57</v>
       </c>
-      <c r="D85" s="212" t="s">
+      <c r="D85" s="214" t="s">
         <v>58</v>
       </c>
-      <c r="E85" s="213" t="s">
+      <c r="E85" s="215" t="s">
         <v>90</v>
       </c>
-      <c r="F85" s="212">
+      <c r="F85" s="214">
         <v>2.0</v>
       </c>
-      <c r="G85" s="227">
+      <c r="G85" s="234"/>
+      <c r="H85" s="233">
         <v>2.0</v>
       </c>
-      <c r="H85" s="210"/>
-      <c r="I85" s="228"/>
-      <c r="J85" s="205"/>
-      <c r="K85" s="206"/>
-      <c r="L85" s="214"/>
-      <c r="M85" s="214"/>
-      <c r="N85" s="214"/>
-      <c r="O85" s="214"/>
-      <c r="P85" s="214"/>
-      <c r="Q85" s="226">
-        <f t="shared" si="18"/>
-        <v>0</v>
+      <c r="I85" s="235"/>
+      <c r="J85" s="207"/>
+      <c r="K85" s="208"/>
+      <c r="L85" s="217">
+        <v>1.0</v>
+      </c>
+      <c r="M85" s="216"/>
+      <c r="N85" s="216"/>
+      <c r="O85" s="216"/>
+      <c r="P85" s="217">
+        <v>1.0</v>
+      </c>
+      <c r="Q85" s="232">
+        <f t="shared" si="20"/>
+        <v>1</v>
       </c>
       <c r="R85" s="177"/>
       <c r="S85" s="177"/>
@@ -5761,54 +5784,54 @@
       <c r="AF85" s="177"/>
     </row>
     <row r="86" ht="12.75" customHeight="1">
-      <c r="A86" s="229" t="s">
+      <c r="A86" s="236" t="s">
         <v>6</v>
       </c>
-      <c r="B86" s="229"/>
-      <c r="C86" s="230"/>
-      <c r="D86" s="230"/>
-      <c r="E86" s="231"/>
-      <c r="F86" s="232">
-        <f t="shared" ref="F86:I86" si="19">SUM(F5:F85)</f>
-        <v>166</v>
-      </c>
-      <c r="G86" s="233">
-        <f t="shared" si="19"/>
-        <v>174</v>
-      </c>
-      <c r="H86" s="232">
-        <f t="shared" si="19"/>
-        <v>114.5</v>
-      </c>
-      <c r="I86" s="233">
-        <f t="shared" si="19"/>
-        <v>114.5</v>
-      </c>
-      <c r="J86" s="234"/>
-      <c r="K86" s="234"/>
-      <c r="L86" s="235">
-        <f t="shared" ref="L86:P86" si="20">SUM(L5:L85)</f>
-        <v>41</v>
-      </c>
-      <c r="M86" s="235">
-        <f t="shared" si="20"/>
-        <v>32</v>
-      </c>
-      <c r="N86" s="235">
-        <f t="shared" si="20"/>
-        <v>24</v>
-      </c>
-      <c r="O86" s="235">
-        <f t="shared" si="20"/>
+      <c r="B86" s="236"/>
+      <c r="C86" s="237"/>
+      <c r="D86" s="237"/>
+      <c r="E86" s="238"/>
+      <c r="F86" s="239">
+        <f t="shared" ref="F86:I86" si="21">SUM(F5:F85)</f>
+        <v>164</v>
+      </c>
+      <c r="G86" s="240">
+        <f t="shared" si="21"/>
+        <v>164</v>
+      </c>
+      <c r="H86" s="239">
+        <f t="shared" si="21"/>
+        <v>144.5</v>
+      </c>
+      <c r="I86" s="240">
+        <f t="shared" si="21"/>
+        <v>144.5</v>
+      </c>
+      <c r="J86" s="177"/>
+      <c r="K86" s="177"/>
+      <c r="L86" s="241">
+        <f t="shared" ref="L86:P86" si="22">SUM(L5:L85)</f>
+        <v>36</v>
+      </c>
+      <c r="M86" s="241">
+        <f t="shared" si="22"/>
+        <v>43</v>
+      </c>
+      <c r="N86" s="241">
+        <f t="shared" si="22"/>
+        <v>28</v>
+      </c>
+      <c r="O86" s="241">
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="P86" s="235">
-        <f t="shared" si="20"/>
-        <v>23.5</v>
-      </c>
-      <c r="Q86" s="235">
+      <c r="P86" s="241">
+        <f t="shared" si="22"/>
+        <v>33.5</v>
+      </c>
+      <c r="Q86" s="241">
         <f>SUM(L86:P86)</f>
-        <v>121.5</v>
+        <v>141.5</v>
       </c>
       <c r="R86" s="177"/>
       <c r="S86" s="177"/>
@@ -5827,23 +5850,23 @@
       <c r="AF86" s="177"/>
     </row>
     <row r="87" ht="12.75" customHeight="1">
-      <c r="A87" s="236"/>
-      <c r="B87" s="236"/>
-      <c r="C87" s="236"/>
-      <c r="D87" s="237"/>
-      <c r="E87" s="236"/>
-      <c r="F87" s="236"/>
-      <c r="G87" s="236"/>
-      <c r="H87" s="236"/>
-      <c r="I87" s="236"/>
-      <c r="J87" s="236"/>
-      <c r="K87" s="236"/>
-      <c r="L87" s="236"/>
-      <c r="M87" s="238"/>
-      <c r="N87" s="238"/>
-      <c r="O87" s="238"/>
-      <c r="P87" s="238"/>
-      <c r="Q87" s="236"/>
+      <c r="A87" s="8"/>
+      <c r="B87" s="8"/>
+      <c r="C87" s="8"/>
+      <c r="D87" s="242"/>
+      <c r="E87" s="8"/>
+      <c r="F87" s="8"/>
+      <c r="G87" s="8"/>
+      <c r="H87" s="8"/>
+      <c r="I87" s="8"/>
+      <c r="J87" s="8"/>
+      <c r="K87" s="8"/>
+      <c r="L87" s="8"/>
+      <c r="M87" s="10"/>
+      <c r="N87" s="10"/>
+      <c r="O87" s="10"/>
+      <c r="P87" s="10"/>
+      <c r="Q87" s="8"/>
       <c r="R87" s="8"/>
       <c r="S87" s="8"/>
       <c r="T87" s="8"/>
@@ -5861,23 +5884,23 @@
       <c r="AF87" s="8"/>
     </row>
     <row r="88" ht="12.75" customHeight="1">
-      <c r="A88" s="236"/>
-      <c r="B88" s="236"/>
-      <c r="C88" s="236"/>
-      <c r="D88" s="237"/>
-      <c r="E88" s="236"/>
-      <c r="F88" s="236"/>
-      <c r="G88" s="236"/>
-      <c r="H88" s="236"/>
-      <c r="I88" s="236"/>
-      <c r="J88" s="236"/>
-      <c r="K88" s="236"/>
-      <c r="L88" s="236"/>
-      <c r="M88" s="238"/>
-      <c r="N88" s="238"/>
-      <c r="O88" s="238"/>
-      <c r="P88" s="238"/>
-      <c r="Q88" s="236"/>
+      <c r="A88" s="8"/>
+      <c r="B88" s="8"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="242"/>
+      <c r="E88" s="8"/>
+      <c r="F88" s="8"/>
+      <c r="G88" s="8"/>
+      <c r="H88" s="8"/>
+      <c r="I88" s="8"/>
+      <c r="J88" s="8"/>
+      <c r="K88" s="8"/>
+      <c r="L88" s="8"/>
+      <c r="M88" s="10"/>
+      <c r="N88" s="10"/>
+      <c r="O88" s="10"/>
+      <c r="P88" s="10"/>
+      <c r="Q88" s="8"/>
       <c r="R88" s="8"/>
       <c r="S88" s="8"/>
       <c r="T88" s="8"/>
@@ -5895,23 +5918,23 @@
       <c r="AF88" s="8"/>
     </row>
     <row r="89" ht="12.75" customHeight="1">
-      <c r="A89" s="236"/>
-      <c r="B89" s="236"/>
-      <c r="C89" s="236"/>
-      <c r="D89" s="237"/>
-      <c r="E89" s="236"/>
-      <c r="F89" s="236"/>
-      <c r="G89" s="236"/>
-      <c r="H89" s="236"/>
-      <c r="I89" s="236"/>
-      <c r="J89" s="236"/>
-      <c r="K89" s="236"/>
-      <c r="L89" s="236"/>
-      <c r="M89" s="238"/>
-      <c r="N89" s="238"/>
-      <c r="O89" s="238"/>
-      <c r="P89" s="238"/>
-      <c r="Q89" s="236"/>
+      <c r="A89" s="8"/>
+      <c r="B89" s="8"/>
+      <c r="C89" s="8"/>
+      <c r="D89" s="242"/>
+      <c r="E89" s="8"/>
+      <c r="F89" s="8"/>
+      <c r="G89" s="8"/>
+      <c r="H89" s="8"/>
+      <c r="I89" s="8"/>
+      <c r="J89" s="8"/>
+      <c r="K89" s="8"/>
+      <c r="L89" s="8"/>
+      <c r="M89" s="10"/>
+      <c r="N89" s="10"/>
+      <c r="O89" s="10"/>
+      <c r="P89" s="10"/>
+      <c r="Q89" s="8"/>
       <c r="R89" s="8"/>
       <c r="S89" s="8"/>
       <c r="T89" s="8"/>
@@ -5929,23 +5952,23 @@
       <c r="AF89" s="8"/>
     </row>
     <row r="90">
-      <c r="A90" s="239"/>
-      <c r="B90" s="239"/>
-      <c r="C90" s="240"/>
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="2"/>
       <c r="D90" s="3"/>
-      <c r="E90" s="241"/>
-      <c r="F90" s="241"/>
-      <c r="G90" s="242"/>
-      <c r="H90" s="241"/>
-      <c r="I90" s="241"/>
-      <c r="J90" s="241"/>
-      <c r="K90" s="241"/>
-      <c r="L90" s="241"/>
-      <c r="M90" s="243"/>
-      <c r="N90" s="243"/>
-      <c r="O90" s="243"/>
-      <c r="P90" s="243"/>
-      <c r="Q90" s="241"/>
+      <c r="E90" s="4"/>
+      <c r="F90" s="4"/>
+      <c r="G90" s="5"/>
+      <c r="H90" s="4"/>
+      <c r="I90" s="4"/>
+      <c r="J90" s="4"/>
+      <c r="K90" s="4"/>
+      <c r="L90" s="4"/>
+      <c r="M90" s="6"/>
+      <c r="N90" s="6"/>
+      <c r="O90" s="6"/>
+      <c r="P90" s="6"/>
+      <c r="Q90" s="4"/>
       <c r="R90" s="4"/>
       <c r="S90" s="4"/>
       <c r="T90" s="4"/>
@@ -5963,23 +5986,23 @@
       <c r="AF90" s="4"/>
     </row>
     <row r="91">
-      <c r="A91" s="239"/>
-      <c r="B91" s="239"/>
-      <c r="C91" s="240"/>
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="2"/>
       <c r="D91" s="3"/>
-      <c r="E91" s="241"/>
-      <c r="F91" s="241"/>
-      <c r="G91" s="242"/>
-      <c r="H91" s="241"/>
-      <c r="I91" s="241"/>
-      <c r="J91" s="241"/>
-      <c r="K91" s="241"/>
-      <c r="L91" s="241"/>
-      <c r="M91" s="243"/>
-      <c r="N91" s="243"/>
-      <c r="O91" s="243"/>
-      <c r="P91" s="243"/>
-      <c r="Q91" s="241"/>
+      <c r="E91" s="4"/>
+      <c r="F91" s="4"/>
+      <c r="G91" s="5"/>
+      <c r="H91" s="4"/>
+      <c r="I91" s="4"/>
+      <c r="J91" s="4"/>
+      <c r="K91" s="4"/>
+      <c r="L91" s="4"/>
+      <c r="M91" s="6"/>
+      <c r="N91" s="6"/>
+      <c r="O91" s="6"/>
+      <c r="P91" s="6"/>
+      <c r="Q91" s="4"/>
       <c r="R91" s="4"/>
       <c r="S91" s="4"/>
       <c r="T91" s="4"/>
@@ -5997,23 +6020,23 @@
       <c r="AF91" s="4"/>
     </row>
     <row r="92">
-      <c r="A92" s="239"/>
-      <c r="B92" s="239"/>
-      <c r="C92" s="240"/>
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="2"/>
       <c r="D92" s="3"/>
-      <c r="E92" s="241"/>
-      <c r="F92" s="241"/>
-      <c r="G92" s="242"/>
-      <c r="H92" s="241"/>
-      <c r="I92" s="241"/>
-      <c r="J92" s="241"/>
-      <c r="K92" s="241"/>
-      <c r="L92" s="241"/>
-      <c r="M92" s="243"/>
-      <c r="N92" s="243"/>
-      <c r="O92" s="243"/>
-      <c r="P92" s="243"/>
-      <c r="Q92" s="241"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="4"/>
+      <c r="G92" s="5"/>
+      <c r="H92" s="4"/>
+      <c r="I92" s="4"/>
+      <c r="J92" s="4"/>
+      <c r="K92" s="4"/>
+      <c r="L92" s="4"/>
+      <c r="M92" s="6"/>
+      <c r="N92" s="6"/>
+      <c r="O92" s="6"/>
+      <c r="P92" s="6"/>
+      <c r="Q92" s="4"/>
       <c r="R92" s="4"/>
       <c r="S92" s="4"/>
       <c r="T92" s="4"/>
@@ -6031,23 +6054,23 @@
       <c r="AF92" s="4"/>
     </row>
     <row r="93">
-      <c r="A93" s="239"/>
-      <c r="B93" s="239"/>
-      <c r="C93" s="240"/>
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="2"/>
       <c r="D93" s="3"/>
-      <c r="E93" s="241"/>
-      <c r="F93" s="241"/>
-      <c r="G93" s="242"/>
-      <c r="H93" s="241"/>
-      <c r="I93" s="241"/>
-      <c r="J93" s="241"/>
-      <c r="K93" s="241"/>
-      <c r="L93" s="241"/>
-      <c r="M93" s="243"/>
-      <c r="N93" s="243"/>
-      <c r="O93" s="243"/>
-      <c r="P93" s="243"/>
-      <c r="Q93" s="241"/>
+      <c r="E93" s="4"/>
+      <c r="F93" s="4"/>
+      <c r="G93" s="5"/>
+      <c r="H93" s="4"/>
+      <c r="I93" s="4"/>
+      <c r="J93" s="4"/>
+      <c r="K93" s="4"/>
+      <c r="L93" s="4"/>
+      <c r="M93" s="6"/>
+      <c r="N93" s="6"/>
+      <c r="O93" s="6"/>
+      <c r="P93" s="6"/>
+      <c r="Q93" s="4"/>
       <c r="R93" s="4"/>
       <c r="S93" s="4"/>
       <c r="T93" s="4"/>
@@ -6065,23 +6088,23 @@
       <c r="AF93" s="4"/>
     </row>
     <row r="94">
-      <c r="A94" s="239"/>
-      <c r="B94" s="239"/>
-      <c r="C94" s="240"/>
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="2"/>
       <c r="D94" s="3"/>
-      <c r="E94" s="241"/>
-      <c r="F94" s="241"/>
-      <c r="G94" s="242"/>
-      <c r="H94" s="241"/>
-      <c r="I94" s="241"/>
-      <c r="J94" s="241"/>
-      <c r="K94" s="241"/>
-      <c r="L94" s="241"/>
-      <c r="M94" s="243"/>
-      <c r="N94" s="243"/>
-      <c r="O94" s="243"/>
-      <c r="P94" s="243"/>
-      <c r="Q94" s="241"/>
+      <c r="E94" s="4"/>
+      <c r="F94" s="4"/>
+      <c r="G94" s="5"/>
+      <c r="H94" s="4"/>
+      <c r="I94" s="4"/>
+      <c r="J94" s="4"/>
+      <c r="K94" s="4"/>
+      <c r="L94" s="4"/>
+      <c r="M94" s="6"/>
+      <c r="N94" s="6"/>
+      <c r="O94" s="6"/>
+      <c r="P94" s="6"/>
+      <c r="Q94" s="4"/>
       <c r="R94" s="4"/>
       <c r="S94" s="4"/>
       <c r="T94" s="4"/>
@@ -6099,23 +6122,23 @@
       <c r="AF94" s="4"/>
     </row>
     <row r="95">
-      <c r="A95" s="239"/>
-      <c r="B95" s="239"/>
-      <c r="C95" s="240"/>
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="2"/>
       <c r="D95" s="3"/>
-      <c r="E95" s="241"/>
-      <c r="F95" s="241"/>
-      <c r="G95" s="242"/>
-      <c r="H95" s="241"/>
-      <c r="I95" s="241"/>
-      <c r="J95" s="241"/>
-      <c r="K95" s="241"/>
-      <c r="L95" s="241"/>
-      <c r="M95" s="243"/>
-      <c r="N95" s="243"/>
-      <c r="O95" s="243"/>
-      <c r="P95" s="243"/>
-      <c r="Q95" s="241"/>
+      <c r="E95" s="4"/>
+      <c r="F95" s="4"/>
+      <c r="G95" s="5"/>
+      <c r="H95" s="4"/>
+      <c r="I95" s="4"/>
+      <c r="J95" s="4"/>
+      <c r="K95" s="4"/>
+      <c r="L95" s="4"/>
+      <c r="M95" s="6"/>
+      <c r="N95" s="6"/>
+      <c r="O95" s="6"/>
+      <c r="P95" s="6"/>
+      <c r="Q95" s="4"/>
       <c r="R95" s="4"/>
       <c r="S95" s="4"/>
       <c r="T95" s="4"/>
@@ -6133,23 +6156,23 @@
       <c r="AF95" s="4"/>
     </row>
     <row r="96">
-      <c r="A96" s="239"/>
-      <c r="B96" s="239"/>
-      <c r="C96" s="240"/>
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="2"/>
       <c r="D96" s="3"/>
-      <c r="E96" s="241"/>
-      <c r="F96" s="241"/>
-      <c r="G96" s="242"/>
-      <c r="H96" s="241"/>
-      <c r="I96" s="241"/>
-      <c r="J96" s="241"/>
-      <c r="K96" s="241"/>
-      <c r="L96" s="241"/>
-      <c r="M96" s="243"/>
-      <c r="N96" s="243"/>
-      <c r="O96" s="243"/>
-      <c r="P96" s="243"/>
-      <c r="Q96" s="241"/>
+      <c r="E96" s="4"/>
+      <c r="F96" s="4"/>
+      <c r="G96" s="5"/>
+      <c r="H96" s="4"/>
+      <c r="I96" s="4"/>
+      <c r="J96" s="4"/>
+      <c r="K96" s="4"/>
+      <c r="L96" s="4"/>
+      <c r="M96" s="6"/>
+      <c r="N96" s="6"/>
+      <c r="O96" s="6"/>
+      <c r="P96" s="6"/>
+      <c r="Q96" s="4"/>
       <c r="R96" s="4"/>
       <c r="S96" s="4"/>
       <c r="T96" s="4"/>

</xml_diff>